<commit_message>
Added Excel Diagrams in Export & new Release
</commit_message>
<xml_diff>
--- a/JSON-Tools/ExcelData/1export_orders.xlsx
+++ b/JSON-Tools/ExcelData/1export_orders.xlsx
@@ -7,160 +7,354 @@
   </x:bookViews>
   <x:sheets>
     <x:sheet name="Export Daten" sheetId="1" r:id="rId2"/>
+    <sheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" name="Dashboard &amp; Analyse" sheetId="2" r:id="rId7"/>
   </x:sheets>
-  <x:definedNames/>
-  <x:calcPr calcId="125725"/>
+  <x:calcPr calcId="125725" fullCalcOnLoad="1"/>
 </x:workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<x:sst xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <x:si>
-    <x:t>ID</x:t>
-  </x:si>
-  <x:si>
-    <x:t>Kunde</x:t>
-  </x:si>
-  <x:si>
-    <x:t>Erstellt</x:t>
-  </x:si>
-  <x:si>
-    <x:t>Gesamtbetrag</x:t>
-  </x:si>
-  <x:si>
-    <x:t>Softline GmbH</x:t>
-  </x:si>
-  <x:si>
-    <x:t>PowerTools KG</x:t>
-  </x:si>
-  <x:si>
-    <x:t>CloudNet GmbH</x:t>
-  </x:si>
-  <x:si>
-    <x:t>Innotech AG</x:t>
-  </x:si>
-  <x:si>
-    <x:t>Bergmann KG</x:t>
-  </x:si>
-  <x:si>
-    <x:t>Alpha GmbH</x:t>
-  </x:si>
-  <x:si>
-    <x:t>TechnoSoft AG</x:t>
-  </x:si>
-  <x:si>
-    <x:t>Delta Systems</x:t>
-  </x:si>
-  <x:si>
-    <x:t>Nordic AG</x:t>
-  </x:si>
-  <x:si>
-    <x:t>Muster GmbH</x:t>
-  </x:si>
-  <x:si>
-    <x:t>Proline GmbH</x:t>
-  </x:si>
-  <x:si>
-    <x:t>Kranbau SE</x:t>
-  </x:si>
-  <x:si>
-    <x:t>Vision IT</x:t>
-  </x:si>
-</x:sst>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="19" uniqueCount="19">
+  <si>
+    <t>Datum</t>
+  </si>
+  <si>
+    <t>Umsatz</t>
+  </si>
+  <si>
+    <t>ID</t>
+  </si>
+  <si>
+    <t>Kunde</t>
+  </si>
+  <si>
+    <t>Erstellt</t>
+  </si>
+  <si>
+    <t>Gesamtbetrag</t>
+  </si>
+  <si>
+    <t>Softline GmbH</t>
+  </si>
+  <si>
+    <t>PowerTools KG</t>
+  </si>
+  <si>
+    <t>CloudNet GmbH</t>
+  </si>
+  <si>
+    <t>Innotech AG</t>
+  </si>
+  <si>
+    <t>Bergmann KG</t>
+  </si>
+  <si>
+    <t>Alpha GmbH</t>
+  </si>
+  <si>
+    <t>TechnoSoft AG</t>
+  </si>
+  <si>
+    <t>Delta Systems</t>
+  </si>
+  <si>
+    <t>Nordic AG</t>
+  </si>
+  <si>
+    <t>Muster GmbH</t>
+  </si>
+  <si>
+    <t>Proline GmbH</t>
+  </si>
+  <si>
+    <t>Kranbau SE</t>
+  </si>
+  <si>
+    <t>Vision IT</t>
+  </si>
+</sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <x:styleSheet xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <x:numFmts count="3">
-    <x:numFmt numFmtId="0" formatCode=""/>
-    <x:numFmt numFmtId="164" formatCode="dd.MM.yyyy"/>
-    <x:numFmt numFmtId="165" formatCode="#,##0.00 €"/>
+    <numFmt xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" numFmtId="0" formatCode=""/>
+    <numFmt xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" numFmtId="164" formatCode="dd.MM.yyyy"/>
+    <numFmt xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" numFmtId="165" formatCode="#,##0.00 €"/>
   </x:numFmts>
   <x:fonts count="2">
-    <x:font>
-      <x:vertAlign val="baseline"/>
-      <x:sz val="11"/>
-      <x:color rgb="FF000000"/>
-      <x:name val="Calibri"/>
-      <x:family val="2"/>
-    </x:font>
-    <x:font>
-      <x:b/>
-      <x:vertAlign val="baseline"/>
-      <x:sz val="11"/>
-      <x:color rgb="FF000000"/>
-      <x:name val="Calibri"/>
-      <x:family val="2"/>
-    </x:font>
+    <font xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+      <d:vertAlign xmlns:d="http://schemas.openxmlformats.org/spreadsheetml/2006/main" val="baseline"/>
+      <d:sz xmlns:d="http://schemas.openxmlformats.org/spreadsheetml/2006/main" val="11"/>
+      <d:color xmlns:d="http://schemas.openxmlformats.org/spreadsheetml/2006/main" rgb="FF000000"/>
+      <d:name xmlns:d="http://schemas.openxmlformats.org/spreadsheetml/2006/main" val="Calibri"/>
+      <d:family xmlns:d="http://schemas.openxmlformats.org/spreadsheetml/2006/main" val="2"/>
+    </font>
+    <font xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+      <d:b xmlns:d="http://schemas.openxmlformats.org/spreadsheetml/2006/main"/>
+      <d:vertAlign xmlns:d="http://schemas.openxmlformats.org/spreadsheetml/2006/main" val="baseline"/>
+      <d:sz xmlns:d="http://schemas.openxmlformats.org/spreadsheetml/2006/main" val="11"/>
+      <d:color xmlns:d="http://schemas.openxmlformats.org/spreadsheetml/2006/main" rgb="FF000000"/>
+      <d:name xmlns:d="http://schemas.openxmlformats.org/spreadsheetml/2006/main" val="Calibri"/>
+      <d:family xmlns:d="http://schemas.openxmlformats.org/spreadsheetml/2006/main" val="2"/>
+    </font>
   </x:fonts>
   <x:fills count="3">
-    <x:fill>
-      <x:patternFill patternType="none"/>
-    </x:fill>
-    <x:fill>
-      <x:patternFill patternType="gray125"/>
-    </x:fill>
-    <x:fill>
-      <x:patternFill patternType="solid">
-        <x:fgColor rgb="FFD3D3D3"/>
-      </x:patternFill>
-    </x:fill>
+    <fill xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+      <d:patternFill xmlns:d="http://schemas.openxmlformats.org/spreadsheetml/2006/main" patternType="none"/>
+    </fill>
+    <fill xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+      <d:patternFill xmlns:d="http://schemas.openxmlformats.org/spreadsheetml/2006/main" patternType="gray125"/>
+    </fill>
+    <fill xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+      <d:patternFill xmlns:d="http://schemas.openxmlformats.org/spreadsheetml/2006/main" patternType="solid">
+        <d:fgColor rgb="FFD3D3D3"/>
+      </d:patternFill>
+    </fill>
   </x:fills>
   <x:borders count="1">
-    <x:border diagonalUp="0" diagonalDown="0">
-      <x:left style="none">
-        <x:color rgb="FF000000"/>
-      </x:left>
-      <x:right style="none">
-        <x:color rgb="FF000000"/>
-      </x:right>
-      <x:top style="none">
-        <x:color rgb="FF000000"/>
-      </x:top>
-      <x:bottom style="none">
-        <x:color rgb="FF000000"/>
-      </x:bottom>
-      <x:diagonal style="none">
-        <x:color rgb="FF000000"/>
-      </x:diagonal>
-    </x:border>
+    <border xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+      <d:left xmlns:d="http://schemas.openxmlformats.org/spreadsheetml/2006/main"/>
+      <d:right xmlns:d="http://schemas.openxmlformats.org/spreadsheetml/2006/main"/>
+      <d:top xmlns:d="http://schemas.openxmlformats.org/spreadsheetml/2006/main"/>
+      <d:bottom xmlns:d="http://schemas.openxmlformats.org/spreadsheetml/2006/main"/>
+      <d:diagonal xmlns:d="http://schemas.openxmlformats.org/spreadsheetml/2006/main"/>
+    </border>
   </x:borders>
-  <x:cellStyleXfs count="4">
-    <x:xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyNumberFormat="1" applyFill="1" applyBorder="0" applyAlignment="1" applyProtection="1">
-      <x:protection locked="1" hidden="0"/>
-    </x:xf>
-    <x:xf numFmtId="0" fontId="1" fillId="2" borderId="0" applyNumberFormat="1" applyFill="0" applyBorder="0" applyAlignment="1" applyProtection="1">
-      <x:protection locked="1" hidden="0"/>
-    </x:xf>
-    <x:xf numFmtId="164" fontId="0" fillId="0" borderId="0" applyNumberFormat="1" applyFill="1" applyBorder="0" applyAlignment="1" applyProtection="1">
-      <x:protection locked="1" hidden="0"/>
-    </x:xf>
-    <x:xf numFmtId="165" fontId="0" fillId="0" borderId="0" applyNumberFormat="1" applyFill="1" applyBorder="0" applyAlignment="1" applyProtection="1">
-      <x:protection locked="1" hidden="0"/>
-    </x:xf>
+  <x:cellStyleXfs count="1">
+    <xf xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </x:cellStyleXfs>
-  <x:cellXfs count="4">
-    <x:xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="0" applyAlignment="1" applyProtection="1">
-      <x:alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="0" indent="0" relativeIndent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-      <x:protection locked="1" hidden="0"/>
-    </x:xf>
-    <x:xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFill="0" applyBorder="0" applyAlignment="1" applyProtection="1">
-      <x:alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="0" indent="0" relativeIndent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-      <x:protection locked="1" hidden="0"/>
-    </x:xf>
-    <x:xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="0" applyAlignment="1" applyProtection="1">
-      <x:alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="0" indent="0" relativeIndent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-      <x:protection locked="1" hidden="0"/>
-    </x:xf>
-    <x:xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="0" applyAlignment="1" applyProtection="1">
-      <x:alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="0" indent="0" relativeIndent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-      <x:protection locked="1" hidden="0"/>
-    </x:xf>
+  <x:cellXfs count="1">
+    <xf xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" numFmtId="0" applyNumberFormat="1" fontId="0" applyFont="1" fillId="0" applyFill="1" borderId="0" applyBorder="1" xfId="0" applyProtection="1"/>
+    <xf xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" numFmtId="0" applyNumberFormat="1" fontId="1" applyFont="1" fillId="2" applyFill="1" borderId="0" applyBorder="1" xfId="0" applyProtection="1"/>
+    <xf xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" numFmtId="164" applyNumberFormat="1" fontId="0" applyFont="1" fillId="0" applyFill="1" borderId="0" applyBorder="1" xfId="0" applyProtection="1"/>
+    <xf xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" numFmtId="165" applyNumberFormat="1" fontId="0" applyFont="1" fillId="0" applyFill="1" borderId="0" applyBorder="1" xfId="0" applyProtection="1"/>
+    <xf xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" numFmtId="164" applyNumberFormat="1" fontId="0" applyFont="1" fillId="0" applyFill="1" borderId="0" applyBorder="1" xfId="0" applyProtection="1"/>
   </x:cellXfs>
   <x:cellStyles count="1">
-    <x:cellStyle name="Normal" xfId="0" builtinId="0"/>
+    <cellStyle xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" name="Normal" xfId="0" builtinId="0"/>
   </x:cellStyles>
 </x:styleSheet>
+</file>
+
+<file path=xl/charts/chart1.xml><?xml version="1.0" encoding="utf-8"?>
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <c:chart>
+    <c:title>
+      <c:tx>
+        <c:rich>
+          <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="1080" b="1" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:effectLst/>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:r>
+              <a:rPr/>
+              <a:t>Täglicher Umsatzverlauf</a:t>
+            </a:r>
+          </a:p>
+        </c:rich>
+      </c:tx>
+      <c:layout/>
+      <c:overlay val="0"/>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+    </c:title>
+    <c:plotArea>
+      <c:layout/>
+      <c:lineChart>
+        <c:grouping val="standard"/>
+        <c:varyColors val="0"/>
+        <c:ser>
+          <c:idx val="0"/>
+          <c:order val="0"/>
+          <c:tx>
+            <c:v>Tagsumsatz</c:v>
+          </c:tx>
+          <c:marker>
+            <c:symbol val="none"/>
+          </c:marker>
+          <c:cat>
+            <c:numRef>
+              <c:f>'Dashboard &amp; Analyse'!$Z$2:$Z$31</c:f>
+            </c:numRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>'Dashboard &amp; Analyse'!$AA$2:$AA$31</c:f>
+              <c:numCache/>
+            </c:numRef>
+          </c:val>
+          <c:smooth val="0"/>
+        </c:ser>
+        <c:smooth val="0"/>
+        <c:axId val="1"/>
+        <c:axId val="2"/>
+      </c:lineChart>
+      <c:catAx>
+        <c:axId val="1"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="b"/>
+        <c:title>
+          <c:tx>
+            <c:rich>
+              <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr sz="1000" b="1" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                    <a:effectLst/>
+                    <a:latin typeface="+mn-lt"/>
+                    <a:ea typeface="+mn-ea"/>
+                    <a:cs typeface="+mn-cs"/>
+                  </a:defRPr>
+                </a:pPr>
+                <a:r>
+                  <a:rPr/>
+                  <a:t>Datum</a:t>
+                </a:r>
+              </a:p>
+            </c:rich>
+          </c:tx>
+          <c:layout/>
+          <c:overlay val="0"/>
+          <c:spPr>
+            <a:noFill/>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+        </c:title>
+        <c:numFmt formatCode="dd.MM.yyyy" sourceLinked="0"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr kern="1200" sz="900"/>
+            </a:pPr>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="2"/>
+        <c:crosses val="autoZero"/>
+        <c:auto val="1"/>
+        <c:lblAlgn val="ctr"/>
+        <c:lblOffset val="100"/>
+      </c:catAx>
+      <c:valAx>
+        <c:axId val="2"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="l"/>
+        <c:majorGridlines/>
+        <c:title>
+          <c:tx>
+            <c:rich>
+              <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr sz="1000" b="1" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                    <a:effectLst/>
+                    <a:latin typeface="+mn-lt"/>
+                    <a:ea typeface="+mn-ea"/>
+                    <a:cs typeface="+mn-cs"/>
+                  </a:defRPr>
+                </a:pPr>
+                <a:r>
+                  <a:rPr/>
+                  <a:t>Umsatz in €</a:t>
+                </a:r>
+              </a:p>
+            </c:rich>
+          </c:tx>
+          <c:layout/>
+          <c:overlay val="0"/>
+          <c:spPr>
+            <a:noFill/>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+        </c:title>
+        <c:numFmt formatCode="#,##0 €" sourceLinked="0"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr kern="1200" sz="900"/>
+            </a:pPr>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="1"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="between"/>
+      </c:valAx>
+    </c:plotArea>
+    <c:plotVisOnly val="1"/>
+  </c:chart>
+  <c:printSettings>
+    <c:headerFooter/>
+    <c:pageMargins b="0.75" l="0.7" r="0.7" t="0.75" header="0.3" footer="0.3"/>
+    <c:pageSetup/>
+  </c:printSettings>
+</c:chartSpace>
+</file>
+
+<file path=xl/drawings/drawing2.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>1</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>1</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>13</xdr:col>
+      <xdr:colOff>304800</xdr:colOff>
+      <xdr:row>21</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:to>
+    <graphicFrame xmlns="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" macro="">
+      <xdr:nvGraphicFramePr>
+        <xdr:cNvPr id="2" name="SalesLineChart"/>
+        <xdr:cNvGraphicFramePr/>
+      </xdr:nvGraphicFramePr>
+      <xdr:xfrm>
+        <a:off x="0" y="0"/>
+        <a:ext cx="0" cy="0"/>
+      </xdr:xfrm>
+      <a:graphic>
+        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
+          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1"/>
+        </a:graphicData>
+      </a:graphic>
+    </graphicFrame>
+    <clientData xmlns="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing"/>
+  </xdr:twoCellAnchor>
+</xdr:wsDr>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -447,7 +641,7 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<x:worksheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main" mc:Ignorable="x14ac">
+<x:worksheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac xr">
   <x:sheetPr>
     <x:outlinePr summaryBelow="1" summaryRight="1"/>
   </x:sheetPr>
@@ -457,46 +651,46 @@
   </x:sheetViews>
   <x:sheetFormatPr defaultRowHeight="15"/>
   <x:cols>
-    <x:col min="1" max="1" width="4.996339" style="0" customWidth="1"/>
-    <x:col min="2" max="2" width="15.424911" style="0" customWidth="1"/>
-    <x:col min="3" max="3" width="10.424911" style="0" customWidth="1"/>
-    <x:col min="4" max="4" width="13.710625" style="0" customWidth="1"/>
+    <x:col min="1" max="1" width="4.996339" customWidth="1"/>
+    <x:col min="2" max="2" width="15.424911" customWidth="1"/>
+    <x:col min="3" max="3" width="10.424911" customWidth="1"/>
+    <x:col min="4" max="4" width="13.710625" customWidth="1"/>
   </x:cols>
   <x:sheetData>
-    <x:row r="1" spans="1:4">
+    <x:row r="1">
       <x:c r="A1" s="1" t="s">
-        <x:v>0</x:v>
+        <x:v>2</x:v>
       </x:c>
       <x:c r="B1" s="1" t="s">
-        <x:v>1</x:v>
+        <x:v>3</x:v>
       </x:c>
       <x:c r="C1" s="1" t="s">
-        <x:v>2</x:v>
+        <x:v>4</x:v>
       </x:c>
       <x:c r="D1" s="1" t="s">
-        <x:v>3</x:v>
-      </x:c>
-    </x:row>
-    <x:row r="2" spans="1:4">
+        <x:v>5</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="2">
       <x:c r="A2" s="0">
         <x:v>2000</x:v>
       </x:c>
       <x:c r="B2" s="0" t="s">
-        <x:v>4</x:v>
+        <x:v>6</x:v>
       </x:c>
       <x:c r="C2" s="2">
         <x:v>45108</x:v>
       </x:c>
       <x:c r="D2" s="3">
-        <x:v>4925.32</x:v>
-      </x:c>
-    </x:row>
-    <x:row r="3" spans="1:4">
+        <x:v>4683.16</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="3">
       <x:c r="A3" s="0">
         <x:v>2001</x:v>
       </x:c>
       <x:c r="B3" s="0" t="s">
-        <x:v>5</x:v>
+        <x:v>7</x:v>
       </x:c>
       <x:c r="C3" s="2">
         <x:v>45109</x:v>
@@ -505,12 +699,12 @@
         <x:v>4683.16</x:v>
       </x:c>
     </x:row>
-    <x:row r="4" spans="1:4">
+    <x:row r="4">
       <x:c r="A4" s="0">
         <x:v>2002</x:v>
       </x:c>
       <x:c r="B4" s="0" t="s">
-        <x:v>5</x:v>
+        <x:v>7</x:v>
       </x:c>
       <x:c r="C4" s="2">
         <x:v>45110</x:v>
@@ -519,12 +713,12 @@
         <x:v>297.89</x:v>
       </x:c>
     </x:row>
-    <x:row r="5" spans="1:4">
+    <x:row r="5">
       <x:c r="A5" s="0">
         <x:v>2003</x:v>
       </x:c>
       <x:c r="B5" s="0" t="s">
-        <x:v>6</x:v>
+        <x:v>8</x:v>
       </x:c>
       <x:c r="C5" s="2">
         <x:v>45111</x:v>
@@ -533,12 +727,12 @@
         <x:v>9626.65</x:v>
       </x:c>
     </x:row>
-    <x:row r="6" spans="1:4">
+    <x:row r="6">
       <x:c r="A6" s="0">
         <x:v>2004</x:v>
       </x:c>
       <x:c r="B6" s="0" t="s">
-        <x:v>7</x:v>
+        <x:v>9</x:v>
       </x:c>
       <x:c r="C6" s="2">
         <x:v>45112</x:v>
@@ -547,12 +741,12 @@
         <x:v>8994.08</x:v>
       </x:c>
     </x:row>
-    <x:row r="7" spans="1:4">
+    <x:row r="7">
       <x:c r="A7" s="0">
         <x:v>2005</x:v>
       </x:c>
       <x:c r="B7" s="0" t="s">
-        <x:v>5</x:v>
+        <x:v>7</x:v>
       </x:c>
       <x:c r="C7" s="2">
         <x:v>45113</x:v>
@@ -561,12 +755,12 @@
         <x:v>3748.5</x:v>
       </x:c>
     </x:row>
-    <x:row r="8" spans="1:4">
+    <x:row r="8">
       <x:c r="A8" s="0">
         <x:v>2006</x:v>
       </x:c>
       <x:c r="B8" s="0" t="s">
-        <x:v>8</x:v>
+        <x:v>10</x:v>
       </x:c>
       <x:c r="C8" s="2">
         <x:v>45114</x:v>
@@ -575,12 +769,12 @@
         <x:v>6159.72</x:v>
       </x:c>
     </x:row>
-    <x:row r="9" spans="1:4">
+    <x:row r="9">
       <x:c r="A9" s="0">
         <x:v>2007</x:v>
       </x:c>
       <x:c r="B9" s="0" t="s">
-        <x:v>9</x:v>
+        <x:v>11</x:v>
       </x:c>
       <x:c r="C9" s="2">
         <x:v>45115</x:v>
@@ -589,12 +783,12 @@
         <x:v>9759.06</x:v>
       </x:c>
     </x:row>
-    <x:row r="10" spans="1:4">
+    <x:row r="10">
       <x:c r="A10" s="0">
         <x:v>2008</x:v>
       </x:c>
       <x:c r="B10" s="0" t="s">
-        <x:v>4</x:v>
+        <x:v>6</x:v>
       </x:c>
       <x:c r="C10" s="2">
         <x:v>45116</x:v>
@@ -603,12 +797,12 @@
         <x:v>4960.17</x:v>
       </x:c>
     </x:row>
-    <x:row r="11" spans="1:4">
+    <x:row r="11">
       <x:c r="A11" s="0">
         <x:v>2009</x:v>
       </x:c>
       <x:c r="B11" s="0" t="s">
-        <x:v>6</x:v>
+        <x:v>8</x:v>
       </x:c>
       <x:c r="C11" s="2">
         <x:v>45117</x:v>
@@ -617,12 +811,12 @@
         <x:v>6405.4</x:v>
       </x:c>
     </x:row>
-    <x:row r="12" spans="1:4">
+    <x:row r="12">
       <x:c r="A12" s="0">
         <x:v>2010</x:v>
       </x:c>
       <x:c r="B12" s="0" t="s">
-        <x:v>7</x:v>
+        <x:v>9</x:v>
       </x:c>
       <x:c r="C12" s="2">
         <x:v>45118</x:v>
@@ -631,12 +825,12 @@
         <x:v>3718.31</x:v>
       </x:c>
     </x:row>
-    <x:row r="13" spans="1:4">
+    <x:row r="13">
       <x:c r="A13" s="0">
         <x:v>2011</x:v>
       </x:c>
       <x:c r="B13" s="0" t="s">
-        <x:v>7</x:v>
+        <x:v>9</x:v>
       </x:c>
       <x:c r="C13" s="2">
         <x:v>45119</x:v>
@@ -645,12 +839,12 @@
         <x:v>9669.53</x:v>
       </x:c>
     </x:row>
-    <x:row r="14" spans="1:4">
+    <x:row r="14">
       <x:c r="A14" s="0">
         <x:v>2012</x:v>
       </x:c>
       <x:c r="B14" s="0" t="s">
-        <x:v>10</x:v>
+        <x:v>12</x:v>
       </x:c>
       <x:c r="C14" s="2">
         <x:v>45120</x:v>
@@ -659,12 +853,12 @@
         <x:v>2341.86</x:v>
       </x:c>
     </x:row>
-    <x:row r="15" spans="1:4">
+    <x:row r="15">
       <x:c r="A15" s="0">
         <x:v>2013</x:v>
       </x:c>
       <x:c r="B15" s="0" t="s">
-        <x:v>11</x:v>
+        <x:v>13</x:v>
       </x:c>
       <x:c r="C15" s="2">
         <x:v>45121</x:v>
@@ -673,12 +867,12 @@
         <x:v>216.34</x:v>
       </x:c>
     </x:row>
-    <x:row r="16" spans="1:4">
+    <x:row r="16">
       <x:c r="A16" s="0">
         <x:v>2014</x:v>
       </x:c>
       <x:c r="B16" s="0" t="s">
-        <x:v>8</x:v>
+        <x:v>10</x:v>
       </x:c>
       <x:c r="C16" s="2">
         <x:v>45122</x:v>
@@ -687,12 +881,12 @@
         <x:v>5395.17</x:v>
       </x:c>
     </x:row>
-    <x:row r="17" spans="1:4">
+    <x:row r="17">
       <x:c r="A17" s="0">
         <x:v>2015</x:v>
       </x:c>
       <x:c r="B17" s="0" t="s">
-        <x:v>4</x:v>
+        <x:v>6</x:v>
       </x:c>
       <x:c r="C17" s="2">
         <x:v>45123</x:v>
@@ -701,12 +895,12 @@
         <x:v>1412.25</x:v>
       </x:c>
     </x:row>
-    <x:row r="18" spans="1:4">
+    <x:row r="18">
       <x:c r="A18" s="0">
         <x:v>2016</x:v>
       </x:c>
       <x:c r="B18" s="0" t="s">
-        <x:v>12</x:v>
+        <x:v>14</x:v>
       </x:c>
       <x:c r="C18" s="2">
         <x:v>45124</x:v>
@@ -715,12 +909,12 @@
         <x:v>689.3</x:v>
       </x:c>
     </x:row>
-    <x:row r="19" spans="1:4">
+    <x:row r="19">
       <x:c r="A19" s="0">
         <x:v>2017</x:v>
       </x:c>
       <x:c r="B19" s="0" t="s">
-        <x:v>7</x:v>
+        <x:v>9</x:v>
       </x:c>
       <x:c r="C19" s="2">
         <x:v>45125</x:v>
@@ -729,12 +923,12 @@
         <x:v>4454.37</x:v>
       </x:c>
     </x:row>
-    <x:row r="20" spans="1:4">
+    <x:row r="20">
       <x:c r="A20" s="0">
         <x:v>2018</x:v>
       </x:c>
       <x:c r="B20" s="0" t="s">
-        <x:v>11</x:v>
+        <x:v>13</x:v>
       </x:c>
       <x:c r="C20" s="2">
         <x:v>45126</x:v>
@@ -743,12 +937,12 @@
         <x:v>3549.96</x:v>
       </x:c>
     </x:row>
-    <x:row r="21" spans="1:4">
+    <x:row r="21">
       <x:c r="A21" s="0">
         <x:v>2019</x:v>
       </x:c>
       <x:c r="B21" s="0" t="s">
-        <x:v>12</x:v>
+        <x:v>14</x:v>
       </x:c>
       <x:c r="C21" s="2">
         <x:v>45127</x:v>
@@ -757,12 +951,12 @@
         <x:v>6917.07</x:v>
       </x:c>
     </x:row>
-    <x:row r="22" spans="1:4">
+    <x:row r="22">
       <x:c r="A22" s="0">
         <x:v>2020</x:v>
       </x:c>
       <x:c r="B22" s="0" t="s">
-        <x:v>6</x:v>
+        <x:v>8</x:v>
       </x:c>
       <x:c r="C22" s="2">
         <x:v>45128</x:v>
@@ -771,12 +965,12 @@
         <x:v>4553.85</x:v>
       </x:c>
     </x:row>
-    <x:row r="23" spans="1:4">
+    <x:row r="23">
       <x:c r="A23" s="0">
         <x:v>2021</x:v>
       </x:c>
       <x:c r="B23" s="0" t="s">
-        <x:v>6</x:v>
+        <x:v>8</x:v>
       </x:c>
       <x:c r="C23" s="2">
         <x:v>45129</x:v>
@@ -785,12 +979,12 @@
         <x:v>4218.03</x:v>
       </x:c>
     </x:row>
-    <x:row r="24" spans="1:4">
+    <x:row r="24">
       <x:c r="A24" s="0">
         <x:v>2022</x:v>
       </x:c>
       <x:c r="B24" s="0" t="s">
-        <x:v>8</x:v>
+        <x:v>10</x:v>
       </x:c>
       <x:c r="C24" s="2">
         <x:v>45130</x:v>
@@ -799,12 +993,12 @@
         <x:v>115.75</x:v>
       </x:c>
     </x:row>
-    <x:row r="25" spans="1:4">
+    <x:row r="25">
       <x:c r="A25" s="0">
         <x:v>2023</x:v>
       </x:c>
       <x:c r="B25" s="0" t="s">
-        <x:v>6</x:v>
+        <x:v>8</x:v>
       </x:c>
       <x:c r="C25" s="2">
         <x:v>45131</x:v>
@@ -813,12 +1007,12 @@
         <x:v>1027.69</x:v>
       </x:c>
     </x:row>
-    <x:row r="26" spans="1:4">
+    <x:row r="26">
       <x:c r="A26" s="0">
         <x:v>2024</x:v>
       </x:c>
       <x:c r="B26" s="0" t="s">
-        <x:v>7</x:v>
+        <x:v>9</x:v>
       </x:c>
       <x:c r="C26" s="2">
         <x:v>45132</x:v>
@@ -827,12 +1021,12 @@
         <x:v>897.34</x:v>
       </x:c>
     </x:row>
-    <x:row r="27" spans="1:4">
+    <x:row r="27">
       <x:c r="A27" s="0">
         <x:v>2025</x:v>
       </x:c>
       <x:c r="B27" s="0" t="s">
-        <x:v>13</x:v>
+        <x:v>15</x:v>
       </x:c>
       <x:c r="C27" s="2">
         <x:v>45133</x:v>
@@ -841,12 +1035,12 @@
         <x:v>3219.96</x:v>
       </x:c>
     </x:row>
-    <x:row r="28" spans="1:4">
+    <x:row r="28">
       <x:c r="A28" s="0">
         <x:v>2026</x:v>
       </x:c>
       <x:c r="B28" s="0" t="s">
-        <x:v>13</x:v>
+        <x:v>15</x:v>
       </x:c>
       <x:c r="C28" s="2">
         <x:v>45134</x:v>
@@ -855,12 +1049,12 @@
         <x:v>431.36</x:v>
       </x:c>
     </x:row>
-    <x:row r="29" spans="1:4">
+    <x:row r="29">
       <x:c r="A29" s="0">
         <x:v>2027</x:v>
       </x:c>
       <x:c r="B29" s="0" t="s">
-        <x:v>14</x:v>
+        <x:v>16</x:v>
       </x:c>
       <x:c r="C29" s="2">
         <x:v>45135</x:v>
@@ -869,12 +1063,12 @@
         <x:v>1600.98</x:v>
       </x:c>
     </x:row>
-    <x:row r="30" spans="1:4">
+    <x:row r="30">
       <x:c r="A30" s="0">
         <x:v>2028</x:v>
       </x:c>
       <x:c r="B30" s="0" t="s">
-        <x:v>4</x:v>
+        <x:v>6</x:v>
       </x:c>
       <x:c r="C30" s="2">
         <x:v>45136</x:v>
@@ -883,12 +1077,12 @@
         <x:v>5396.71</x:v>
       </x:c>
     </x:row>
-    <x:row r="31" spans="1:4">
+    <x:row r="31">
       <x:c r="A31" s="0">
         <x:v>2029</x:v>
       </x:c>
       <x:c r="B31" s="0" t="s">
-        <x:v>14</x:v>
+        <x:v>16</x:v>
       </x:c>
       <x:c r="C31" s="2">
         <x:v>45137</x:v>
@@ -897,12 +1091,12 @@
         <x:v>9575.96</x:v>
       </x:c>
     </x:row>
-    <x:row r="32" spans="1:4">
+    <x:row r="32">
       <x:c r="A32" s="0">
         <x:v>2030</x:v>
       </x:c>
       <x:c r="B32" s="0" t="s">
-        <x:v>14</x:v>
+        <x:v>16</x:v>
       </x:c>
       <x:c r="C32" s="2">
         <x:v>45108</x:v>
@@ -911,12 +1105,12 @@
         <x:v>566.59</x:v>
       </x:c>
     </x:row>
-    <x:row r="33" spans="1:4">
+    <x:row r="33">
       <x:c r="A33" s="0">
         <x:v>2031</x:v>
       </x:c>
       <x:c r="B33" s="0" t="s">
-        <x:v>9</x:v>
+        <x:v>11</x:v>
       </x:c>
       <x:c r="C33" s="2">
         <x:v>45109</x:v>
@@ -925,12 +1119,12 @@
         <x:v>1036.12</x:v>
       </x:c>
     </x:row>
-    <x:row r="34" spans="1:4">
+    <x:row r="34">
       <x:c r="A34" s="0">
         <x:v>2032</x:v>
       </x:c>
       <x:c r="B34" s="0" t="s">
-        <x:v>13</x:v>
+        <x:v>15</x:v>
       </x:c>
       <x:c r="C34" s="2">
         <x:v>45110</x:v>
@@ -939,12 +1133,12 @@
         <x:v>7079.78</x:v>
       </x:c>
     </x:row>
-    <x:row r="35" spans="1:4">
+    <x:row r="35">
       <x:c r="A35" s="0">
         <x:v>2033</x:v>
       </x:c>
       <x:c r="B35" s="0" t="s">
-        <x:v>15</x:v>
+        <x:v>17</x:v>
       </x:c>
       <x:c r="C35" s="2">
         <x:v>45111</x:v>
@@ -953,12 +1147,12 @@
         <x:v>1831.16</x:v>
       </x:c>
     </x:row>
-    <x:row r="36" spans="1:4">
+    <x:row r="36">
       <x:c r="A36" s="0">
         <x:v>2034</x:v>
       </x:c>
       <x:c r="B36" s="0" t="s">
-        <x:v>15</x:v>
+        <x:v>17</x:v>
       </x:c>
       <x:c r="C36" s="2">
         <x:v>45112</x:v>
@@ -967,12 +1161,12 @@
         <x:v>6321.76</x:v>
       </x:c>
     </x:row>
-    <x:row r="37" spans="1:4">
+    <x:row r="37">
       <x:c r="A37" s="0">
         <x:v>2035</x:v>
       </x:c>
       <x:c r="B37" s="0" t="s">
-        <x:v>10</x:v>
+        <x:v>12</x:v>
       </x:c>
       <x:c r="C37" s="2">
         <x:v>45113</x:v>
@@ -981,12 +1175,12 @@
         <x:v>424.37</x:v>
       </x:c>
     </x:row>
-    <x:row r="38" spans="1:4">
+    <x:row r="38">
       <x:c r="A38" s="0">
         <x:v>2036</x:v>
       </x:c>
       <x:c r="B38" s="0" t="s">
-        <x:v>12</x:v>
+        <x:v>14</x:v>
       </x:c>
       <x:c r="C38" s="2">
         <x:v>45114</x:v>
@@ -995,12 +1189,12 @@
         <x:v>2892.66</x:v>
       </x:c>
     </x:row>
-    <x:row r="39" spans="1:4">
+    <x:row r="39">
       <x:c r="A39" s="0">
         <x:v>2037</x:v>
       </x:c>
       <x:c r="B39" s="0" t="s">
-        <x:v>7</x:v>
+        <x:v>9</x:v>
       </x:c>
       <x:c r="C39" s="2">
         <x:v>45115</x:v>
@@ -1009,12 +1203,12 @@
         <x:v>9816.36</x:v>
       </x:c>
     </x:row>
-    <x:row r="40" spans="1:4">
+    <x:row r="40">
       <x:c r="A40" s="0">
         <x:v>2038</x:v>
       </x:c>
       <x:c r="B40" s="0" t="s">
-        <x:v>8</x:v>
+        <x:v>10</x:v>
       </x:c>
       <x:c r="C40" s="2">
         <x:v>45116</x:v>
@@ -1023,12 +1217,12 @@
         <x:v>5705.71</x:v>
       </x:c>
     </x:row>
-    <x:row r="41" spans="1:4">
+    <x:row r="41">
       <x:c r="A41" s="0">
         <x:v>2039</x:v>
       </x:c>
       <x:c r="B41" s="0" t="s">
-        <x:v>11</x:v>
+        <x:v>13</x:v>
       </x:c>
       <x:c r="C41" s="2">
         <x:v>45117</x:v>
@@ -1037,12 +1231,12 @@
         <x:v>2380.58</x:v>
       </x:c>
     </x:row>
-    <x:row r="42" spans="1:4">
+    <x:row r="42">
       <x:c r="A42" s="0">
         <x:v>2040</x:v>
       </x:c>
       <x:c r="B42" s="0" t="s">
-        <x:v>13</x:v>
+        <x:v>15</x:v>
       </x:c>
       <x:c r="C42" s="2">
         <x:v>45118</x:v>
@@ -1051,12 +1245,12 @@
         <x:v>4575.97</x:v>
       </x:c>
     </x:row>
-    <x:row r="43" spans="1:4">
+    <x:row r="43">
       <x:c r="A43" s="0">
         <x:v>2041</x:v>
       </x:c>
       <x:c r="B43" s="0" t="s">
-        <x:v>5</x:v>
+        <x:v>7</x:v>
       </x:c>
       <x:c r="C43" s="2">
         <x:v>45119</x:v>
@@ -1065,12 +1259,12 @@
         <x:v>8175.6</x:v>
       </x:c>
     </x:row>
-    <x:row r="44" spans="1:4">
+    <x:row r="44">
       <x:c r="A44" s="0">
         <x:v>2042</x:v>
       </x:c>
       <x:c r="B44" s="0" t="s">
-        <x:v>9</x:v>
+        <x:v>11</x:v>
       </x:c>
       <x:c r="C44" s="2">
         <x:v>45120</x:v>
@@ -1079,12 +1273,12 @@
         <x:v>9813.8</x:v>
       </x:c>
     </x:row>
-    <x:row r="45" spans="1:4">
+    <x:row r="45">
       <x:c r="A45" s="0">
         <x:v>2043</x:v>
       </x:c>
       <x:c r="B45" s="0" t="s">
-        <x:v>13</x:v>
+        <x:v>15</x:v>
       </x:c>
       <x:c r="C45" s="2">
         <x:v>45121</x:v>
@@ -1093,12 +1287,12 @@
         <x:v>8841.37</x:v>
       </x:c>
     </x:row>
-    <x:row r="46" spans="1:4">
+    <x:row r="46">
       <x:c r="A46" s="0">
         <x:v>2044</x:v>
       </x:c>
       <x:c r="B46" s="0" t="s">
-        <x:v>11</x:v>
+        <x:v>13</x:v>
       </x:c>
       <x:c r="C46" s="2">
         <x:v>45122</x:v>
@@ -1107,12 +1301,12 @@
         <x:v>4439.52</x:v>
       </x:c>
     </x:row>
-    <x:row r="47" spans="1:4">
+    <x:row r="47">
       <x:c r="A47" s="0">
         <x:v>2045</x:v>
       </x:c>
       <x:c r="B47" s="0" t="s">
-        <x:v>13</x:v>
+        <x:v>15</x:v>
       </x:c>
       <x:c r="C47" s="2">
         <x:v>45123</x:v>
@@ -1121,12 +1315,12 @@
         <x:v>8738.76</x:v>
       </x:c>
     </x:row>
-    <x:row r="48" spans="1:4">
+    <x:row r="48">
       <x:c r="A48" s="0">
         <x:v>2046</x:v>
       </x:c>
       <x:c r="B48" s="0" t="s">
-        <x:v>15</x:v>
+        <x:v>17</x:v>
       </x:c>
       <x:c r="C48" s="2">
         <x:v>45124</x:v>
@@ -1135,12 +1329,12 @@
         <x:v>8080.55</x:v>
       </x:c>
     </x:row>
-    <x:row r="49" spans="1:4">
+    <x:row r="49">
       <x:c r="A49" s="0">
         <x:v>2047</x:v>
       </x:c>
       <x:c r="B49" s="0" t="s">
-        <x:v>6</x:v>
+        <x:v>8</x:v>
       </x:c>
       <x:c r="C49" s="2">
         <x:v>45125</x:v>
@@ -1149,12 +1343,12 @@
         <x:v>4064.46</x:v>
       </x:c>
     </x:row>
-    <x:row r="50" spans="1:4">
+    <x:row r="50">
       <x:c r="A50" s="0">
         <x:v>2048</x:v>
       </x:c>
       <x:c r="B50" s="0" t="s">
-        <x:v>7</x:v>
+        <x:v>9</x:v>
       </x:c>
       <x:c r="C50" s="2">
         <x:v>45126</x:v>
@@ -1163,12 +1357,12 @@
         <x:v>9280.79</x:v>
       </x:c>
     </x:row>
-    <x:row r="51" spans="1:4">
+    <x:row r="51">
       <x:c r="A51" s="0">
         <x:v>2049</x:v>
       </x:c>
       <x:c r="B51" s="0" t="s">
-        <x:v>16</x:v>
+        <x:v>18</x:v>
       </x:c>
       <x:c r="C51" s="2">
         <x:v>45127</x:v>
@@ -1184,4 +1378,269 @@
   <x:headerFooter/>
   <x:tableParts count="0"/>
 </x:worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" mc:Ignorable="xr">
+  <dimension ref="Z1:AA31"/>
+  <sheetViews>
+    <sheetView workbookViewId="0"/>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15"/>
+  <cols>
+    <col min="26" max="26" width="9.140625" customWidth="1" style="4"/>
+  </cols>
+  <sheetData>
+    <row r="1">
+      <c r="Z1" s="4" t="s">
+        <v>0</v>
+      </c>
+      <c r="AA1" s="0" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="2">
+      <c r="Z2" s="4">
+        <v>45108</v>
+      </c>
+      <c r="AA2" s="0">
+        <v>5249.75</v>
+      </c>
+    </row>
+    <row r="3">
+      <c r="Z3" s="4">
+        <v>45109</v>
+      </c>
+      <c r="AA3" s="0">
+        <v>5719.28</v>
+      </c>
+    </row>
+    <row r="4">
+      <c r="Z4" s="4">
+        <v>45110</v>
+      </c>
+      <c r="AA4" s="0">
+        <v>7377.67</v>
+      </c>
+    </row>
+    <row r="5">
+      <c r="Z5" s="4">
+        <v>45111</v>
+      </c>
+      <c r="AA5" s="0">
+        <v>11457.81</v>
+      </c>
+    </row>
+    <row r="6">
+      <c r="Z6" s="4">
+        <v>45112</v>
+      </c>
+      <c r="AA6" s="0">
+        <v>15315.84</v>
+      </c>
+    </row>
+    <row r="7">
+      <c r="Z7" s="4">
+        <v>45113</v>
+      </c>
+      <c r="AA7" s="0">
+        <v>4172.87</v>
+      </c>
+    </row>
+    <row r="8">
+      <c r="Z8" s="4">
+        <v>45114</v>
+      </c>
+      <c r="AA8" s="0">
+        <v>9052.38</v>
+      </c>
+    </row>
+    <row r="9">
+      <c r="Z9" s="4">
+        <v>45115</v>
+      </c>
+      <c r="AA9" s="0">
+        <v>19575.42</v>
+      </c>
+    </row>
+    <row r="10">
+      <c r="Z10" s="4">
+        <v>45116</v>
+      </c>
+      <c r="AA10" s="0">
+        <v>10665.88</v>
+      </c>
+    </row>
+    <row r="11">
+      <c r="Z11" s="4">
+        <v>45117</v>
+      </c>
+      <c r="AA11" s="0">
+        <v>8785.98</v>
+      </c>
+    </row>
+    <row r="12">
+      <c r="Z12" s="4">
+        <v>45118</v>
+      </c>
+      <c r="AA12" s="0">
+        <v>8294.28</v>
+      </c>
+    </row>
+    <row r="13">
+      <c r="Z13" s="4">
+        <v>45119</v>
+      </c>
+      <c r="AA13" s="0">
+        <v>17845.13</v>
+      </c>
+    </row>
+    <row r="14">
+      <c r="Z14" s="4">
+        <v>45120</v>
+      </c>
+      <c r="AA14" s="0">
+        <v>12155.66</v>
+      </c>
+    </row>
+    <row r="15">
+      <c r="Z15" s="4">
+        <v>45121</v>
+      </c>
+      <c r="AA15" s="0">
+        <v>9057.71</v>
+      </c>
+    </row>
+    <row r="16">
+      <c r="Z16" s="4">
+        <v>45122</v>
+      </c>
+      <c r="AA16" s="0">
+        <v>9834.69</v>
+      </c>
+    </row>
+    <row r="17">
+      <c r="Z17" s="4">
+        <v>45123</v>
+      </c>
+      <c r="AA17" s="0">
+        <v>10151.01</v>
+      </c>
+    </row>
+    <row r="18">
+      <c r="Z18" s="4">
+        <v>45124</v>
+      </c>
+      <c r="AA18" s="0">
+        <v>8769.85</v>
+      </c>
+    </row>
+    <row r="19">
+      <c r="Z19" s="4">
+        <v>45125</v>
+      </c>
+      <c r="AA19" s="0">
+        <v>8518.83</v>
+      </c>
+    </row>
+    <row r="20">
+      <c r="Z20" s="4">
+        <v>45126</v>
+      </c>
+      <c r="AA20" s="0">
+        <v>12830.75</v>
+      </c>
+    </row>
+    <row r="21">
+      <c r="Z21" s="4">
+        <v>45127</v>
+      </c>
+      <c r="AA21" s="0">
+        <v>7054.81</v>
+      </c>
+    </row>
+    <row r="22">
+      <c r="Z22" s="4">
+        <v>45128</v>
+      </c>
+      <c r="AA22" s="0">
+        <v>4553.85</v>
+      </c>
+    </row>
+    <row r="23">
+      <c r="Z23" s="4">
+        <v>45129</v>
+      </c>
+      <c r="AA23" s="0">
+        <v>4218.03</v>
+      </c>
+    </row>
+    <row r="24">
+      <c r="Z24" s="4">
+        <v>45130</v>
+      </c>
+      <c r="AA24" s="0">
+        <v>115.75</v>
+      </c>
+    </row>
+    <row r="25">
+      <c r="Z25" s="4">
+        <v>45131</v>
+      </c>
+      <c r="AA25" s="0">
+        <v>1027.69</v>
+      </c>
+    </row>
+    <row r="26">
+      <c r="Z26" s="4">
+        <v>45132</v>
+      </c>
+      <c r="AA26" s="0">
+        <v>897.34</v>
+      </c>
+    </row>
+    <row r="27">
+      <c r="Z27" s="4">
+        <v>45133</v>
+      </c>
+      <c r="AA27" s="0">
+        <v>3219.96</v>
+      </c>
+    </row>
+    <row r="28">
+      <c r="Z28" s="4">
+        <v>45134</v>
+      </c>
+      <c r="AA28" s="0">
+        <v>431.36</v>
+      </c>
+    </row>
+    <row r="29">
+      <c r="Z29" s="4">
+        <v>45135</v>
+      </c>
+      <c r="AA29" s="0">
+        <v>1600.98</v>
+      </c>
+    </row>
+    <row r="30">
+      <c r="Z30" s="4">
+        <v>45136</v>
+      </c>
+      <c r="AA30" s="0">
+        <v>5396.71</v>
+      </c>
+    </row>
+    <row r="31">
+      <c r="Z31" s="4">
+        <v>45137</v>
+      </c>
+      <c r="AA31" s="0">
+        <v>9575.96</v>
+      </c>
+    </row>
+  </sheetData>
+  <headerFooter/>
+  <drawing r:id="rId1"/>
+</worksheet>
 </file>
</xml_diff>